<commit_message>
feat: Add sorting by creation date in card import functionality
</commit_message>
<xml_diff>
--- a/ZiTyLot/Resource/Excel-templates/Card-template.xlsx
+++ b/ZiTyLot/Resource/Excel-templates/Card-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoBui\Desktop\CSharp\ZiTyLot\ZiTyLot\Resource\Excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoBui\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F55587-CF20-4ECE-8EA9-486B98734B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA1B1C-68E6-48E4-B3A3-161B213CAB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3612" yWindow="3156" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -50,6 +50,11 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,12 +77,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -417,19 +432,20 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="5" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -446,140 +462,140 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>

</xml_diff>